<commit_message>
Added target practise scene, stopped them falling under gravity and started looking into creating an OnCollisionCallback to change theur colour when hit.
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Physics</t>
   </si>
@@ -77,10 +77,22 @@
     <t>Make Target Scene</t>
   </si>
   <si>
-    <t>Make them move with a spring constraint when hit</t>
-  </si>
-  <si>
     <t>GPU ACCELERATION</t>
+  </si>
+  <si>
+    <t>Collision Response</t>
+  </si>
+  <si>
+    <t>Display Number of Entities</t>
+  </si>
+  <si>
+    <t>Implement rest states</t>
+  </si>
+  <si>
+    <t>Use lambda to change colour</t>
+  </si>
+  <si>
+    <t>Add spring constraint</t>
   </si>
 </sst>
 </file>
@@ -180,14 +192,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,12 +528,11 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="5" t="s">
-        <v>12</v>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -531,58 +545,91 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>6</v>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G5" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F5" s="2" t="s">
+      <c r="H5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
+      <c r="G6" s="3"/>
+      <c r="H6" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
         <v>16</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F7" s="2" t="s">
+      <c r="G10" s="3"/>
+      <c r="H10" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H8" s="1" t="s">
+      <c r="H11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="8" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Completed basic target scene, with spring constraints and changing colours.
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>Physics</t>
   </si>
@@ -96,6 +96,30 @@
   </si>
   <si>
     <t>May need to make Target class that inherits from GameObject with timer and 'hit' bool</t>
+  </si>
+  <si>
+    <t>Debug draw spring</t>
+  </si>
+  <si>
+    <t>Make the line several lines making up a jagged triagnle spring constraint</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>SOFT BODY</t>
+  </si>
+  <si>
+    <t>Make spring constr generic</t>
+  </si>
+  <si>
+    <t>If necessary</t>
+  </si>
+  <si>
+    <t>Change Performance timers</t>
+  </si>
+  <si>
+    <t>Add in broadphase and narrowphase like in the tutorials</t>
   </si>
 </sst>
 </file>
@@ -111,7 +135,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,6 +154,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -195,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -206,6 +236,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,28 +610,28 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F6" s="2" t="s">
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>6</v>
+      <c r="G7" s="3"/>
+      <c r="H7" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>12</v>
@@ -608,34 +639,76 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F10" s="2" t="s">
+      <c r="H10" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="6" t="s">
+      <c r="G12" s="3"/>
+      <c r="H12" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F11" s="5" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F12" s="5" t="s">
+      <c r="H13" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H14" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="8" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added in empty soft body scene
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Physics</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Add in broadphase and narrowphase like in the tutorials</t>
+  </si>
+  <si>
+    <t>COMPOUND SHAPES</t>
+  </si>
+  <si>
+    <t>SATISFACTORY</t>
   </si>
 </sst>
 </file>
@@ -135,7 +141,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,6 +166,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -235,8 +247,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,7 +541,8 @@
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="6" max="6" width="26.85546875" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="9" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -625,8 +638,8 @@
         <v>15</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="6" t="s">
-        <v>12</v>
+      <c r="H7" s="10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -634,7 +647,7 @@
         <v>16</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -644,7 +657,7 @@
       <c r="G9" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -652,7 +665,7 @@
       <c r="F10" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -709,6 +722,15 @@
         <v>29</v>
       </c>
       <c r="H16" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="7" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed spring copnstraints and implemented a rudimentary softy body, with as yet no texturing.
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>Physics</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>SATISFACTORY</t>
+  </si>
+  <si>
+    <t>When a projectile is fired - increment entity, when an object falls out of octree, decrement</t>
   </si>
 </sst>
 </file>
@@ -237,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -247,6 +250,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -532,7 +536,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +642,7 @@
         <v>15</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="11" t="s">
         <v>33</v>
       </c>
     </row>
@@ -646,7 +650,7 @@
       <c r="F8" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="10" t="s">
         <v>26</v>
       </c>
     </row>
@@ -657,7 +661,7 @@
       <c r="G9" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="10" t="s">
         <v>26</v>
       </c>
     </row>
@@ -665,7 +669,7 @@
       <c r="F10" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="10" t="s">
         <v>26</v>
       </c>
     </row>
@@ -701,8 +705,11 @@
       <c r="F14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="8" t="s">
-        <v>6</v>
+      <c r="G14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Made rendernode mesh for colouring the softbody
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>Physics</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Make spring constr generic</t>
   </si>
   <si>
-    <t>If necessary</t>
-  </si>
-  <si>
     <t>Change Performance timers</t>
   </si>
   <si>
@@ -129,6 +126,24 @@
   </si>
   <si>
     <t>When a projectile is fired - increment entity, when an object falls out of octree, decrement</t>
+  </si>
+  <si>
+    <t>Doesn't have any angular conditions</t>
+  </si>
+  <si>
+    <t>Generate a texturable mesh</t>
+  </si>
+  <si>
+    <t>Don't cull back faces</t>
+  </si>
+  <si>
+    <t>Don't collide with itself</t>
+  </si>
+  <si>
+    <t>Make soft body class</t>
+  </si>
+  <si>
+    <t>Make draggable</t>
   </si>
 </sst>
 </file>
@@ -240,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -253,6 +268,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,10 +644,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
         <v>30</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>6</v>
@@ -643,7 +659,7 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -706,7 +722,7 @@
         <v>19</v>
       </c>
       <c r="G14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>12</v>
@@ -717,8 +733,8 @@
         <v>27</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="7" t="s">
-        <v>6</v>
+      <c r="H15" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -726,18 +742,58 @@
         <v>28</v>
       </c>
       <c r="G16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>6</v>
+        <v>34</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="7" t="s">
+      <c r="F17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F21" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="7" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Integrated physics code from physics coursework into network coursework.
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
   <si>
     <t>Physics</t>
   </si>
@@ -144,6 +144,15 @@
   </si>
   <si>
     <t>Make draggable</t>
+  </si>
+  <si>
+    <t>Networks</t>
+  </si>
+  <si>
+    <t>Create an outofbound check</t>
+  </si>
+  <si>
+    <t>Rermoves need for expensive floor/ wall collision check</t>
   </si>
 </sst>
 </file>
@@ -549,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,9 +572,10 @@
     <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="15.140625" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -584,8 +594,17 @@
       <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -602,7 +621,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -620,7 +639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>10</v>
       </c>
@@ -631,7 +650,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>14</v>
       </c>
@@ -642,7 +661,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>29</v>
       </c>
@@ -653,7 +672,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F7" s="2" t="s">
         <v>15</v>
       </c>
@@ -662,7 +681,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>16</v>
       </c>
@@ -670,7 +689,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
         <v>21</v>
       </c>
@@ -681,7 +700,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>22</v>
       </c>
@@ -689,7 +708,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>24</v>
       </c>
@@ -700,7 +719,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F12" s="2" t="s">
         <v>17</v>
       </c>
@@ -709,7 +728,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F13" s="5" t="s">
         <v>18</v>
       </c>
@@ -717,7 +736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F14" s="5" t="s">
         <v>19</v>
       </c>
@@ -728,45 +747,48 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F15" s="2" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="6" t="s">
+      <c r="G16" s="3"/>
+      <c r="H16" s="6" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="17" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>12</v>
+        <v>28</v>
+      </c>
+      <c r="G17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F18" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>6</v>
+        <v>35</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F19" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>6</v>
@@ -774,26 +796,34 @@
     </row>
     <row r="20" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F20" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="21" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F22" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F22" s="2" t="s">
+      <c r="H22" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="7" t="s">
+      <c r="G23" s="3"/>
+      <c r="H23" s="7" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added in the 'NetworkEntity' class to encapsulate the client and server packet handling functionality.
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
   <si>
     <t>Physics</t>
   </si>
@@ -153,6 +153,30 @@
   </si>
   <si>
     <t>Rermoves need for expensive floor/ wall collision check</t>
+  </si>
+  <si>
+    <t>Merge projects</t>
+  </si>
+  <si>
+    <t>Get server to generate maze</t>
+  </si>
+  <si>
+    <t>Promote Client to server</t>
+  </si>
+  <si>
+    <t>When a server disconnects, make a client the server</t>
+  </si>
+  <si>
+    <t>Get server to send maze back</t>
+  </si>
+  <si>
+    <t>Get client to print out maze</t>
+  </si>
+  <si>
+    <t>Create server and client classes</t>
+  </si>
+  <si>
+    <t>Tidy up the code a bit</t>
   </si>
 </sst>
 </file>
@@ -264,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -278,6 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,7 +586,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +597,9 @@
     <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="15.140625" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" customWidth="1"/>
+    <col min="11" max="11" width="34.42578125" customWidth="1"/>
+    <col min="12" max="12" width="23" customWidth="1"/>
+    <col min="13" max="13" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -620,6 +647,12 @@
       <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="K2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -638,6 +671,12 @@
       <c r="H3" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="K3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
@@ -649,6 +688,15 @@
       <c r="H4" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="K4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
@@ -660,6 +708,12 @@
       <c r="H5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="K5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
@@ -671,6 +725,12 @@
       <c r="H6" s="8" t="s">
         <v>6</v>
       </c>
+      <c r="K6" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F7" s="2" t="s">
@@ -679,6 +739,15 @@
       <c r="G7" s="3"/>
       <c r="H7" s="11" t="s">
         <v>32</v>
+      </c>
+      <c r="K7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L7" t="s">
+        <v>50</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed packets from structs to classes, made a abstract Packet base class the MazeRequest and MazeData packets inherit. Each class has a CreateByteStream method that returns a pointer to an array of enet_uint8's (unsigned chars) for easier transmitting of packets.
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="54">
   <si>
     <t>Physics</t>
   </si>
@@ -177,6 +177,15 @@
   </si>
   <si>
     <t>Tidy up the code a bit</t>
+  </si>
+  <si>
+    <t>Make user able to exit server</t>
+  </si>
+  <si>
+    <t>By hitting 'esc'</t>
+  </si>
+  <si>
+    <t>Get client to receive messages</t>
   </si>
 </sst>
 </file>
@@ -288,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -303,6 +312,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,7 +596,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,8 +721,11 @@
       <c r="K5" t="s">
         <v>47</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>6</v>
+      <c r="L5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -756,6 +769,15 @@
       </c>
       <c r="H8" s="10" t="s">
         <v>26</v>
+      </c>
+      <c r="K8" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8" t="s">
+        <v>52</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Server transmits maze data to client, client reconstructs maze at client side.
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -185,7 +185,7 @@
     <t>By hitting 'esc'</t>
   </si>
   <si>
-    <t>Get client to receive messages</t>
+    <t>Change transmit method to stream of booleans instead</t>
   </si>
 </sst>
 </file>
@@ -297,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -313,6 +313,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,7 +597,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,8 +725,8 @@
       <c r="L5" t="s">
         <v>53</v>
       </c>
-      <c r="M5" s="14" t="s">
-        <v>12</v>
+      <c r="M5" s="15" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -741,8 +742,8 @@
       <c r="K6" t="s">
         <v>48</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>6</v>
+      <c r="M6" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Maze data now sent as boolean data - saving on transmission time
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="55">
   <si>
     <t>Physics</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>Change transmit method to stream of booleans instead</t>
+  </si>
+  <si>
+    <t>Allow user input</t>
   </si>
 </sst>
 </file>
@@ -297,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -313,7 +316,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,7 +599,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,8 +727,8 @@
       <c r="L5" t="s">
         <v>53</v>
       </c>
-      <c r="M5" s="15" t="s">
-        <v>32</v>
+      <c r="M5" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -790,6 +792,12 @@
       </c>
       <c r="H9" s="10" t="s">
         <v>26</v>
+      </c>
+      <c r="K9" t="s">
+        <v>54</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Correct maze reformed at client side
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -300,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -315,7 +315,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -744,8 +743,8 @@
       <c r="K6" t="s">
         <v>48</v>
       </c>
-      <c r="M6" s="14" t="s">
-        <v>12</v>
+      <c r="M6" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
User input added to change basic maze parameters
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
   <si>
     <t>Physics</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>Allow user input</t>
+  </si>
+  <si>
+    <t>Solve memory issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> when adding half a byte</t>
   </si>
 </sst>
 </file>
@@ -598,7 +604,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,8 +801,8 @@
       <c r="K9" t="s">
         <v>54</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>6</v>
+      <c r="M9" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -805,6 +811,15 @@
       </c>
       <c r="H10" s="10" t="s">
         <v>26</v>
+      </c>
+      <c r="K10" t="s">
+        <v>55</v>
+      </c>
+      <c r="L10" t="s">
+        <v>56</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Sorted the packet class structure headers to make them more organised. Also added the client replying to the server with its start and end positions.
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
   <si>
     <t>Physics</t>
   </si>
@@ -195,6 +195,27 @@
   </si>
   <si>
     <t xml:space="preserve"> when adding half a byte</t>
+  </si>
+  <si>
+    <t>Display current maze size as well as user input maze size to be requested</t>
+  </si>
+  <si>
+    <t>Transmit start and end position</t>
+  </si>
+  <si>
+    <t>from client to server</t>
+  </si>
+  <si>
+    <t>Accept position &amp; compute route</t>
+  </si>
+  <si>
+    <t>Add options client side for different types of algorithm</t>
+  </si>
+  <si>
+    <t>Send route back to client</t>
+  </si>
+  <si>
+    <t>Client should display route on key press</t>
   </si>
 </sst>
 </file>
@@ -604,7 +625,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="M11" activeCellId="1" sqref="M10 M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,6 +822,9 @@
       <c r="K9" t="s">
         <v>54</v>
       </c>
+      <c r="L9" t="s">
+        <v>57</v>
+      </c>
       <c r="M9" s="13" t="s">
         <v>26</v>
       </c>
@@ -818,8 +842,8 @@
       <c r="L10" t="s">
         <v>56</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>6</v>
+      <c r="M10" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -832,6 +856,15 @@
       <c r="H11" s="8" t="s">
         <v>6</v>
       </c>
+      <c r="K11" t="s">
+        <v>58</v>
+      </c>
+      <c r="L11" t="s">
+        <v>59</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F12" s="2" t="s">
@@ -841,12 +874,30 @@
       <c r="H12" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="K12" t="s">
+        <v>60</v>
+      </c>
+      <c r="L12" t="s">
+        <v>61</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F13" s="5" t="s">
         <v>18</v>
       </c>
       <c r="H13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" t="s">
+        <v>62</v>
+      </c>
+      <c r="L13" t="s">
+        <v>63</v>
+      </c>
+      <c r="M13" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Server computes A* path for client, client stores it as array of integer indices into maze->allNodes array. Client can draw the path.
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
   <si>
     <t>Physics</t>
   </si>
@@ -197,9 +197,6 @@
     <t xml:space="preserve"> when adding half a byte</t>
   </si>
   <si>
-    <t>Display current maze size as well as user input maze size to be requested</t>
-  </si>
-  <si>
     <t>Transmit start and end position</t>
   </si>
   <si>
@@ -216,6 +213,18 @@
   </si>
   <si>
     <t>Client should display route on key press</t>
+  </si>
+  <si>
+    <t>Allow user to resize the dimensions of the maze</t>
+  </si>
+  <si>
+    <t>User move start/ end position</t>
+  </si>
+  <si>
+    <t>Server console output</t>
+  </si>
+  <si>
+    <t>For each different packet</t>
   </si>
 </sst>
 </file>
@@ -625,7 +634,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" activeCellId="1" sqref="M10 M11"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,10 +832,10 @@
         <v>54</v>
       </c>
       <c r="L9" t="s">
-        <v>57</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>26</v>
+        <v>63</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -857,10 +866,10 @@
         <v>6</v>
       </c>
       <c r="K11" t="s">
+        <v>57</v>
+      </c>
+      <c r="L11" t="s">
         <v>58</v>
-      </c>
-      <c r="L11" t="s">
-        <v>59</v>
       </c>
       <c r="M11" s="13" t="s">
         <v>26</v>
@@ -875,13 +884,13 @@
         <v>12</v>
       </c>
       <c r="K12" t="s">
+        <v>59</v>
+      </c>
+      <c r="L12" t="s">
         <v>60</v>
       </c>
-      <c r="L12" t="s">
-        <v>61</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>6</v>
+      <c r="M12" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -892,13 +901,13 @@
         <v>6</v>
       </c>
       <c r="K13" t="s">
+        <v>61</v>
+      </c>
+      <c r="L13" t="s">
         <v>62</v>
       </c>
-      <c r="L13" t="s">
-        <v>63</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>6</v>
+      <c r="M13" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -911,6 +920,12 @@
       <c r="H14" s="9" t="s">
         <v>12</v>
       </c>
+      <c r="K14" t="s">
+        <v>64</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F15" s="5" t="s">
@@ -920,6 +935,15 @@
         <v>42</v>
       </c>
       <c r="H15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" t="s">
+        <v>65</v>
+      </c>
+      <c r="L15" t="s">
+        <v>66</v>
+      </c>
+      <c r="M15" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changing structure of code. Make NetworkEntity class just a packet handler, changed Net1_Client name to Client and going to create a Server class that stores a vector of Client structs with info about their ID, start/ end position, paths etc.
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="70">
   <si>
     <t>Physics</t>
   </si>
@@ -225,6 +225,15 @@
   </si>
   <si>
     <t>For each different packet</t>
+  </si>
+  <si>
+    <t>Create client avatar</t>
+  </si>
+  <si>
+    <t>Change when new start/end positions sent</t>
+  </si>
+  <si>
+    <t>Send on keypress</t>
   </si>
 </sst>
 </file>
@@ -634,7 +643,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,8 +964,14 @@
       <c r="H16" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>67</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F17" s="5" t="s">
         <v>28</v>
       </c>
@@ -966,8 +981,17 @@
       <c r="H17" s="12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>68</v>
+      </c>
+      <c r="L17" t="s">
+        <v>69</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F18" s="5" t="s">
         <v>35</v>
       </c>
@@ -975,7 +999,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F19" s="5" t="s">
         <v>36</v>
       </c>
@@ -983,7 +1007,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F20" s="5" t="s">
         <v>37</v>
       </c>
@@ -991,7 +1015,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F21" s="5" t="s">
         <v>38</v>
       </c>
@@ -999,7 +1023,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F22" s="5" t="s">
         <v>39</v>
       </c>
@@ -1007,7 +1031,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F23" s="2" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Stores maze start and end index to make moving positions more efficient. Began implementing a InstructionReceived packet.
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="74">
   <si>
     <t>Physics</t>
   </si>
@@ -234,6 +234,18 @@
   </si>
   <si>
     <t>Send on keypress</t>
+  </si>
+  <si>
+    <t>Remove rotating box</t>
+  </si>
+  <si>
+    <t>Clean up code used to handle this</t>
+  </si>
+  <si>
+    <t>Add "CONNECTED" status entry</t>
+  </si>
+  <si>
+    <t>Or "NOT CONNECTED"</t>
   </si>
 </sst>
 </file>
@@ -643,7 +655,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,12 +1010,30 @@
       <c r="H18" s="9" t="s">
         <v>12</v>
       </c>
+      <c r="K18" t="s">
+        <v>70</v>
+      </c>
+      <c r="L18" t="s">
+        <v>71</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="19" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F19" s="5" t="s">
         <v>36</v>
       </c>
       <c r="H19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19" t="s">
+        <v>72</v>
+      </c>
+      <c r="L19" t="s">
+        <v>73</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New clients can now receive mazes of any size as the server will send them the maze parameters and maze data upon joining the network.
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="75">
   <si>
     <t>Physics</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>Or "NOT CONNECTED"</t>
+  </si>
+  <si>
+    <t>Add keypress to reconnect</t>
   </si>
 </sst>
 </file>
@@ -655,7 +658,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,8 +1002,8 @@
       <c r="L17" t="s">
         <v>69</v>
       </c>
-      <c r="M17" s="1" t="s">
-        <v>6</v>
+      <c r="M17" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="6:13" x14ac:dyDescent="0.25">
@@ -1042,6 +1045,12 @@
         <v>37</v>
       </c>
       <c r="H20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" t="s">
+        <v>74</v>
+      </c>
+      <c r="M20" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Client avatar now tarces its pathy from start to end node then stops. The pysics for this is carried out on the server side
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="79">
   <si>
     <t>Physics</t>
   </si>
@@ -249,6 +249,18 @@
   </si>
   <si>
     <t>Add keypress to reconnect</t>
+  </si>
+  <si>
+    <t>Allow client to run</t>
+  </si>
+  <si>
+    <t>Increase their avatar's speed</t>
+  </si>
+  <si>
+    <t>Move avatar at server end</t>
+  </si>
+  <si>
+    <t>Display other client's avatars</t>
   </si>
 </sst>
 </file>
@@ -658,7 +670,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,8 +994,8 @@
       <c r="K16" t="s">
         <v>67</v>
       </c>
-      <c r="M16" s="1" t="s">
-        <v>6</v>
+      <c r="M16" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="6:13" x14ac:dyDescent="0.25">
@@ -997,10 +1009,7 @@
         <v>32</v>
       </c>
       <c r="K17" t="s">
-        <v>68</v>
-      </c>
-      <c r="L17" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="M17" s="13" t="s">
         <v>26</v>
@@ -1014,13 +1023,13 @@
         <v>12</v>
       </c>
       <c r="K18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L18" t="s">
-        <v>71</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>6</v>
+        <v>69</v>
+      </c>
+      <c r="M18" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="6:13" x14ac:dyDescent="0.25">
@@ -1031,10 +1040,10 @@
         <v>6</v>
       </c>
       <c r="K19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>6</v>
@@ -1048,7 +1057,10 @@
         <v>6</v>
       </c>
       <c r="K20" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="L20" t="s">
+        <v>73</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>6</v>
@@ -1061,6 +1073,12 @@
       <c r="H21" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="K21" t="s">
+        <v>74</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="22" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F22" s="5" t="s">
@@ -1069,6 +1087,15 @@
       <c r="H22" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="K22" t="s">
+        <v>75</v>
+      </c>
+      <c r="L22" t="s">
+        <v>76</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="23" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F23" s="2" t="s">
@@ -1076,6 +1103,12 @@
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" t="s">
+        <v>78</v>
+      </c>
+      <c r="M23" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Avatar position and path updates when a maze is regenerated. Avatar position calculated by physicsengine.
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="86">
   <si>
     <t>Physics</t>
   </si>
@@ -273,6 +273,15 @@
   </si>
   <si>
     <t xml:space="preserve">IS BROKEN </t>
+  </si>
+  <si>
+    <t>UsePhysics bool</t>
+  </si>
+  <si>
+    <t>Allow client to change whether their position is calculated in the physics engine or not - include in ConnecetedClient struct</t>
+  </si>
+  <si>
+    <t>R BUTTON ??</t>
   </si>
 </sst>
 </file>
@@ -679,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,8 +1097,11 @@
       <c r="K21" t="s">
         <v>74</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>6</v>
+      <c r="L21" t="s">
+        <v>85</v>
+      </c>
+      <c r="M21" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="6:13" x14ac:dyDescent="0.25">
@@ -1131,8 +1143,8 @@
       <c r="L24" t="s">
         <v>80</v>
       </c>
-      <c r="M24" s="1" t="s">
-        <v>6</v>
+      <c r="M24" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="6:13" x14ac:dyDescent="0.25">
@@ -1142,7 +1154,18 @@
       <c r="L25" t="s">
         <v>82</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="M25" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>83</v>
+      </c>
+      <c r="L26" t="s">
+        <v>84</v>
+      </c>
+      <c r="M26" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Physics engine position doesn't work 100% so there is an option for the client to choose how their position is calculated.
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="89">
   <si>
     <t>Physics</t>
   </si>
@@ -282,6 +282,15 @@
   </si>
   <si>
     <t>R BUTTON ??</t>
+  </si>
+  <si>
+    <t>Move start position with avatar</t>
+  </si>
+  <si>
+    <t>Change end position</t>
+  </si>
+  <si>
+    <t>Without reposistioning avatar</t>
   </si>
 </sst>
 </file>
@@ -688,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,7 +1174,26 @@
       <c r="L26" t="s">
         <v>84</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="M26" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>86</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>87</v>
+      </c>
+      <c r="L28" t="s">
+        <v>88</v>
+      </c>
+      <c r="M28" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Can now change avatar position and resend position packet and the avatar will not jump to the start position. It will continue on its path
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="90">
   <si>
     <t>Physics</t>
   </si>
@@ -287,10 +287,13 @@
     <t>Move start position with avatar</t>
   </si>
   <si>
-    <t>Change end position</t>
-  </si>
-  <si>
-    <t>Without reposistioning avatar</t>
+    <t>Stop avatar jumping around</t>
+  </si>
+  <si>
+    <t>Change end without reposistioning avatar</t>
+  </si>
+  <si>
+    <t>Change start without moving avatar</t>
   </si>
 </sst>
 </file>
@@ -697,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,6 +1200,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="29" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="L29" t="s">
+        <v>89</v>
+      </c>
+      <c r="M29" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed the way the client changes its positions. Now the user can change the goal node and the server will recalculate the path from the avatar's current position. If the start node is moved, a whole new path is calculated.
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="91">
   <si>
     <t>Physics</t>
   </si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t>Change start without moving avatar</t>
+  </si>
+  <si>
+    <t>Make it look like it is consuming the path</t>
   </si>
 </sst>
 </file>
@@ -703,7 +706,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,6 +1188,9 @@
       <c r="K27" t="s">
         <v>86</v>
       </c>
+      <c r="L27" t="s">
+        <v>90</v>
+      </c>
       <c r="M27" s="1" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Clients can now see other connected cleints' avatars
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="93">
   <si>
     <t>Physics</t>
   </si>
@@ -296,7 +296,13 @@
     <t>Change start without moving avatar</t>
   </si>
   <si>
-    <t>Make it look like it is consuming the path</t>
+    <t>Needs to look smoother</t>
+  </si>
+  <si>
+    <t>When reaches destination</t>
+  </si>
+  <si>
+    <t>Change start to avatar location</t>
   </si>
 </sst>
 </file>
@@ -703,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,8 +1153,8 @@
       <c r="K23" t="s">
         <v>78</v>
       </c>
-      <c r="M23" s="1" t="s">
-        <v>6</v>
+      <c r="M23" s="9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="6:13" x14ac:dyDescent="0.25">
@@ -1191,8 +1197,8 @@
       <c r="L27" t="s">
         <v>90</v>
       </c>
-      <c r="M27" s="1" t="s">
-        <v>6</v>
+      <c r="M27" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="6:13" x14ac:dyDescent="0.25">
@@ -1202,8 +1208,8 @@
       <c r="L28" t="s">
         <v>88</v>
       </c>
-      <c r="M28" s="1" t="s">
-        <v>6</v>
+      <c r="M28" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="6:13" x14ac:dyDescent="0.25">
@@ -1212,6 +1218,17 @@
       </c>
       <c r="M29" s="13" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>91</v>
+      </c>
+      <c r="L30" t="s">
+        <v>92</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct client avatar colours, and when a client regenerates the maze, the avatars all respawn as well.
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="97">
   <si>
     <t>Physics</t>
   </si>
@@ -303,6 +303,18 @@
   </si>
   <si>
     <t>Change start to avatar location</t>
+  </si>
+  <si>
+    <t>Correct avatar colours</t>
+  </si>
+  <si>
+    <t>Blue for you</t>
+  </si>
+  <si>
+    <t>Increment balls in pool</t>
+  </si>
+  <si>
+    <t>Have a Window::KeyTrigger capture in the scene class</t>
   </si>
 </sst>
 </file>
@@ -709,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,12 +1038,14 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="6" t="s">
-        <v>12</v>
+      <c r="F16" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16" t="s">
+        <v>96</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="K16" t="s">
         <v>67</v>
@@ -1041,14 +1055,12 @@
       </c>
     </row>
     <row r="17" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>32</v>
+      <c r="F17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="K17" t="s">
         <v>77</v>
@@ -1059,10 +1071,13 @@
     </row>
     <row r="18" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F18" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>12</v>
+        <v>28</v>
+      </c>
+      <c r="G18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="K18" t="s">
         <v>68</v>
@@ -1076,10 +1091,10 @@
     </row>
     <row r="19" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>6</v>
+        <v>35</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="K19" t="s">
         <v>70</v>
@@ -1093,7 +1108,7 @@
     </row>
     <row r="20" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F20" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>6</v>
@@ -1110,9 +1125,9 @@
     </row>
     <row r="21" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="8" t="s">
         <v>6</v>
       </c>
       <c r="K21" t="s">
@@ -1127,7 +1142,7 @@
     </row>
     <row r="22" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F22" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>6</v>
@@ -1143,11 +1158,10 @@
       </c>
     </row>
     <row r="23" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="7" t="s">
+      <c r="F23" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K23" t="s">
@@ -1158,6 +1172,13 @@
       </c>
     </row>
     <row r="24" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="3"/>
+      <c r="H24" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="K24" t="s">
         <v>79</v>
       </c>
@@ -1229,6 +1250,17 @@
       </c>
       <c r="M30" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>93</v>
+      </c>
+      <c r="L31" t="s">
+        <v>94</v>
+      </c>
+      <c r="M31" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented a string pulling algorithm to minimise the number of nodes necessary to traverse in a path.
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="99">
   <si>
     <t>Physics</t>
   </si>
@@ -315,6 +315,12 @@
   </si>
   <si>
     <t>Have a Window::KeyTrigger capture in the scene class</t>
+  </si>
+  <si>
+    <t>String pulling</t>
+  </si>
+  <si>
+    <t>Recalculate routes after toggling</t>
   </si>
 </sst>
 </file>
@@ -721,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,8 +1173,8 @@
       <c r="K23" t="s">
         <v>78</v>
       </c>
-      <c r="M23" s="9" t="s">
-        <v>12</v>
+      <c r="M23" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="6:13" x14ac:dyDescent="0.25">
@@ -1261,6 +1267,17 @@
       </c>
       <c r="M31" s="13" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>97</v>
+      </c>
+      <c r="L32" t="s">
+        <v>98</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started making ball pool better
</commit_message>
<xml_diff>
--- a/GameTech/TODO.xlsx
+++ b/GameTech/TODO.xlsx
@@ -729,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,8 +1013,8 @@
       <c r="G14" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="9" t="s">
-        <v>12</v>
+      <c r="H14" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="K14" t="s">
         <v>64</v>
@@ -1050,8 +1050,8 @@
       <c r="G16" t="s">
         <v>96</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>6</v>
+      <c r="H16" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="K16" t="s">
         <v>67</v>
@@ -1116,8 +1116,8 @@
       <c r="F20" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H20" s="8" t="s">
-        <v>6</v>
+      <c r="H20" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="K20" t="s">
         <v>72</v>
@@ -1167,8 +1167,8 @@
       <c r="F23" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>6</v>
+      <c r="H23" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="K23" t="s">
         <v>78</v>

</xml_diff>